<commit_message>
Revised Estimation : Reverted DB Schema
</commit_message>
<xml_diff>
--- a/Database Schema Fantasylab.xlsx
+++ b/Database Schema Fantasylab.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9302"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="600" windowWidth="20490" windowHeight="7155"/>
+    <workbookView xWindow="0" yWindow="660" windowWidth="20490" windowHeight="7095"/>
   </bookViews>
   <sheets>
     <sheet name="Schema" sheetId="1" r:id="rId1"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="626" uniqueCount="89">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="585" uniqueCount="84">
   <si>
     <t>No</t>
   </si>
@@ -267,22 +267,7 @@
     <t>fantasylab</t>
   </si>
   <si>
-    <t>p_projects</t>
-  </si>
-  <si>
-    <t>p_title</t>
-  </si>
-  <si>
-    <t>p_department</t>
-  </si>
-  <si>
-    <t>p_website</t>
-  </si>
-  <si>
-    <t>p_type</t>
-  </si>
-  <si>
-    <t>1-Featured, 2-Inprogress</t>
+    <t>fl_d_departments</t>
   </si>
 </sst>
 </file>
@@ -511,7 +496,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="51">
+  <cellXfs count="46">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -619,20 +604,14 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" indent="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -646,19 +625,10 @@
     <xf numFmtId="0" fontId="2" fillId="5" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -965,10 +935,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K462"/>
+  <dimension ref="A1:K465"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="C10" sqref="C10"/>
+      <selection activeCell="A3" sqref="A3:K3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -988,283 +958,175 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="42" t="s">
+      <c r="A1" s="40" t="s">
         <v>81</v>
       </c>
-      <c r="B1" s="42"/>
-      <c r="C1" s="42"/>
-      <c r="D1" s="42"/>
-      <c r="E1" s="42"/>
-      <c r="F1" s="42"/>
-      <c r="G1" s="42"/>
-      <c r="H1" s="42"/>
-      <c r="I1" s="42"/>
-      <c r="J1" s="42"/>
-      <c r="K1" s="42"/>
+      <c r="B1" s="40"/>
+      <c r="C1" s="40"/>
+      <c r="D1" s="40"/>
+      <c r="E1" s="40"/>
+      <c r="F1" s="40"/>
+      <c r="G1" s="40"/>
+      <c r="H1" s="40"/>
+      <c r="I1" s="40"/>
+      <c r="J1" s="40"/>
+      <c r="K1" s="40"/>
     </row>
     <row r="2" spans="1:11" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="43" t="s">
+      <c r="A2" s="41" t="s">
         <v>82</v>
       </c>
-      <c r="B2" s="44"/>
-      <c r="C2" s="44"/>
-      <c r="D2" s="44"/>
-      <c r="E2" s="44"/>
-      <c r="F2" s="44"/>
-      <c r="G2" s="44"/>
-      <c r="H2" s="44"/>
-      <c r="I2" s="44"/>
-      <c r="J2" s="44"/>
-      <c r="K2" s="45"/>
+      <c r="B2" s="42"/>
+      <c r="C2" s="42"/>
+      <c r="D2" s="42"/>
+      <c r="E2" s="42"/>
+      <c r="F2" s="42"/>
+      <c r="G2" s="42"/>
+      <c r="H2" s="42"/>
+      <c r="I2" s="42"/>
+      <c r="J2" s="42"/>
+      <c r="K2" s="43"/>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A3" s="46" t="s">
+      <c r="A3" s="37" t="s">
         <v>83</v>
       </c>
-      <c r="B3" s="47"/>
-      <c r="C3" s="47"/>
-      <c r="D3" s="47"/>
-      <c r="E3" s="47"/>
-      <c r="F3" s="47"/>
-      <c r="G3" s="47"/>
-      <c r="H3" s="47"/>
-      <c r="I3" s="47"/>
-      <c r="J3" s="47"/>
-      <c r="K3" s="48"/>
+      <c r="B3" s="38"/>
+      <c r="C3" s="38"/>
+      <c r="D3" s="38"/>
+      <c r="E3" s="38"/>
+      <c r="F3" s="38"/>
+      <c r="G3" s="38"/>
+      <c r="H3" s="38"/>
+      <c r="I3" s="38"/>
+      <c r="J3" s="38"/>
+      <c r="K3" s="39"/>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A4" s="19" t="s">
+      <c r="A4" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="B4" s="18" t="s">
+      <c r="B4" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="C4" s="18" t="s">
+      <c r="C4" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="D4" s="18" t="s">
+      <c r="D4" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="E4" s="18" t="s">
+      <c r="E4" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="F4" s="18" t="s">
+      <c r="F4" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="G4" s="18" t="s">
+      <c r="G4" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="H4" s="18" t="s">
+      <c r="H4" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="I4" s="19" t="s">
+      <c r="I4" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="J4" s="19" t="s">
+      <c r="J4" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="K4" s="18" t="s">
+      <c r="K4" s="4" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A5" s="28">
-        <v>1</v>
-      </c>
-      <c r="B5" s="5" t="s">
-        <v>25</v>
-      </c>
-      <c r="C5" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="D5" s="5">
-        <v>10</v>
-      </c>
-      <c r="E5" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="F5" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="G5" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="H5" s="5" t="s">
-        <v>0</v>
-      </c>
-      <c r="I5" s="37" t="s">
-        <v>12</v>
-      </c>
-      <c r="J5" s="37"/>
-      <c r="K5" s="6" t="s">
-        <v>13</v>
-      </c>
+      <c r="A5" s="7"/>
+      <c r="B5" s="7"/>
+      <c r="C5" s="7"/>
+      <c r="D5" s="7"/>
+      <c r="E5" s="7"/>
+      <c r="F5" s="7"/>
+      <c r="G5" s="7"/>
+      <c r="H5" s="7"/>
+      <c r="I5" s="7"/>
+      <c r="J5" s="7"/>
+      <c r="K5" s="7"/>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A6" s="39">
-        <v>2</v>
-      </c>
-      <c r="B6" s="7" t="s">
-        <v>84</v>
-      </c>
-      <c r="C6" s="7" t="s">
-        <v>14</v>
-      </c>
-      <c r="D6" s="7">
-        <v>255</v>
-      </c>
+      <c r="A6" s="7"/>
+      <c r="B6" s="7"/>
+      <c r="C6" s="7"/>
+      <c r="D6" s="7"/>
       <c r="E6" s="7"/>
-      <c r="F6" s="7" t="s">
-        <v>10</v>
-      </c>
+      <c r="F6" s="7"/>
       <c r="G6" s="7"/>
-      <c r="H6" s="7" t="s">
-        <v>0</v>
-      </c>
+      <c r="H6" s="7"/>
       <c r="I6" s="7"/>
-      <c r="J6" s="7" t="s">
-        <v>12</v>
-      </c>
-      <c r="K6" s="9"/>
+      <c r="J6" s="7"/>
+      <c r="K6" s="7"/>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A7" s="39">
-        <v>3</v>
-      </c>
-      <c r="B7" s="7" t="s">
-        <v>85</v>
-      </c>
-      <c r="C7" s="7" t="s">
-        <v>14</v>
-      </c>
-      <c r="D7" s="7">
-        <v>255</v>
-      </c>
+      <c r="A7" s="7"/>
+      <c r="B7" s="7"/>
+      <c r="C7" s="7"/>
+      <c r="D7" s="7"/>
       <c r="E7" s="7"/>
-      <c r="F7" s="7" t="s">
-        <v>10</v>
-      </c>
+      <c r="F7" s="7"/>
       <c r="G7" s="7"/>
-      <c r="H7" s="7" t="s">
-        <v>0</v>
-      </c>
+      <c r="H7" s="7"/>
       <c r="I7" s="7"/>
-      <c r="J7" s="7" t="s">
-        <v>12</v>
-      </c>
-      <c r="K7" s="9"/>
+      <c r="J7" s="7"/>
+      <c r="K7" s="7"/>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A8" s="39">
-        <v>4</v>
-      </c>
-      <c r="B8" s="7" t="s">
-        <v>86</v>
-      </c>
-      <c r="C8" s="7" t="s">
-        <v>14</v>
-      </c>
-      <c r="D8" s="7">
-        <v>100</v>
-      </c>
+      <c r="A8" s="7"/>
+      <c r="B8" s="7"/>
+      <c r="C8" s="7"/>
+      <c r="D8" s="7"/>
       <c r="E8" s="7"/>
-      <c r="F8" s="7" t="s">
-        <v>10</v>
-      </c>
+      <c r="F8" s="7"/>
       <c r="G8" s="7"/>
-      <c r="H8" s="7" t="s">
-        <v>0</v>
-      </c>
+      <c r="H8" s="7"/>
       <c r="I8" s="7"/>
-      <c r="J8" s="7" t="s">
-        <v>12</v>
-      </c>
-      <c r="K8" s="9"/>
+      <c r="J8" s="7"/>
+      <c r="K8" s="7"/>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A9" s="39">
-        <v>5</v>
-      </c>
-      <c r="B9" s="7" t="s">
-        <v>87</v>
-      </c>
-      <c r="C9" s="7" t="s">
-        <v>15</v>
-      </c>
-      <c r="D9" s="7">
-        <v>1</v>
-      </c>
+      <c r="A9" s="7"/>
+      <c r="B9" s="7"/>
+      <c r="C9" s="7"/>
+      <c r="D9" s="7"/>
       <c r="E9" s="7"/>
-      <c r="F9" s="7">
-        <v>1</v>
-      </c>
-      <c r="G9" s="7" t="s">
-        <v>11</v>
-      </c>
-      <c r="H9" s="7" t="s">
-        <v>0</v>
-      </c>
+      <c r="F9" s="7"/>
+      <c r="G9" s="7"/>
+      <c r="H9" s="7"/>
       <c r="I9" s="7"/>
-      <c r="J9" s="7" t="s">
-        <v>12</v>
-      </c>
-      <c r="K9" s="9" t="s">
-        <v>88</v>
-      </c>
+      <c r="J9" s="7"/>
+      <c r="K9" s="7"/>
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A10" s="39">
-        <v>6</v>
-      </c>
-      <c r="B10" s="7" t="s">
-        <v>23</v>
-      </c>
-      <c r="C10" s="7" t="s">
-        <v>17</v>
-      </c>
+      <c r="A10" s="7"/>
+      <c r="B10" s="7"/>
+      <c r="C10" s="7"/>
       <c r="D10" s="7"/>
-      <c r="E10" s="12" t="s">
-        <v>26</v>
-      </c>
-      <c r="F10" s="12" t="s">
-        <v>26</v>
-      </c>
+      <c r="E10" s="7"/>
+      <c r="F10" s="7"/>
       <c r="G10" s="7"/>
-      <c r="H10" s="7" t="s">
-        <v>12</v>
-      </c>
-      <c r="I10" s="36"/>
-      <c r="J10" s="36"/>
-      <c r="K10" s="9" t="s">
-        <v>16</v>
-      </c>
+      <c r="H10" s="7"/>
+      <c r="I10" s="7"/>
+      <c r="J10" s="7"/>
+      <c r="K10" s="7"/>
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A11" s="40">
-        <v>7</v>
-      </c>
-      <c r="B11" s="13" t="s">
-        <v>24</v>
-      </c>
-      <c r="C11" s="13" t="s">
-        <v>17</v>
-      </c>
-      <c r="D11" s="13"/>
-      <c r="E11" s="41" t="s">
-        <v>18</v>
-      </c>
-      <c r="F11" s="41" t="s">
-        <v>18</v>
-      </c>
-      <c r="G11" s="13"/>
-      <c r="H11" s="13" t="s">
-        <v>12</v>
-      </c>
-      <c r="I11" s="38"/>
-      <c r="J11" s="38"/>
-      <c r="K11" s="14" t="s">
-        <v>16</v>
-      </c>
+      <c r="A11" s="7"/>
+      <c r="B11" s="7"/>
+      <c r="C11" s="7"/>
+      <c r="D11" s="7"/>
+      <c r="E11" s="7"/>
+      <c r="F11" s="7"/>
+      <c r="G11" s="7"/>
+      <c r="H11" s="7"/>
+      <c r="I11" s="7"/>
+      <c r="J11" s="7"/>
+      <c r="K11" s="7"/>
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A12" s="7"/>
@@ -1903,7 +1765,7 @@
       <c r="J60" s="7"/>
       <c r="K60" s="7"/>
     </row>
-    <row r="61" spans="1:11" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A61" s="7"/>
       <c r="B61" s="7"/>
       <c r="C61" s="7"/>
@@ -1916,7 +1778,7 @@
       <c r="J61" s="7"/>
       <c r="K61" s="7"/>
     </row>
-    <row r="62" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:11" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A62" s="7"/>
       <c r="B62" s="7"/>
       <c r="C62" s="7"/>
@@ -1942,7 +1804,7 @@
       <c r="J63" s="7"/>
       <c r="K63" s="7"/>
     </row>
-    <row r="64" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A64" s="7"/>
       <c r="B64" s="7"/>
       <c r="C64" s="7"/>
@@ -1955,7 +1817,7 @@
       <c r="J64" s="7"/>
       <c r="K64" s="7"/>
     </row>
-    <row r="65" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A65" s="7"/>
       <c r="B65" s="7"/>
       <c r="C65" s="7"/>
@@ -7128,6 +6990,45 @@
       <c r="I462" s="7"/>
       <c r="J462" s="7"/>
       <c r="K462" s="7"/>
+    </row>
+    <row r="463" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A463" s="7"/>
+      <c r="B463" s="7"/>
+      <c r="C463" s="7"/>
+      <c r="D463" s="7"/>
+      <c r="E463" s="7"/>
+      <c r="F463" s="7"/>
+      <c r="G463" s="7"/>
+      <c r="H463" s="7"/>
+      <c r="I463" s="7"/>
+      <c r="J463" s="7"/>
+      <c r="K463" s="7"/>
+    </row>
+    <row r="464" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A464" s="7"/>
+      <c r="B464" s="7"/>
+      <c r="C464" s="7"/>
+      <c r="D464" s="7"/>
+      <c r="E464" s="7"/>
+      <c r="F464" s="7"/>
+      <c r="G464" s="7"/>
+      <c r="H464" s="7"/>
+      <c r="I464" s="7"/>
+      <c r="J464" s="7"/>
+      <c r="K464" s="7"/>
+    </row>
+    <row r="465" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A465" s="7"/>
+      <c r="B465" s="7"/>
+      <c r="C465" s="7"/>
+      <c r="D465" s="7"/>
+      <c r="E465" s="7"/>
+      <c r="F465" s="7"/>
+      <c r="G465" s="7"/>
+      <c r="H465" s="7"/>
+      <c r="I465" s="7"/>
+      <c r="J465" s="7"/>
+      <c r="K465" s="7"/>
     </row>
   </sheetData>
   <mergeCells count="3">
@@ -7205,45 +7106,45 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A1" s="49"/>
-      <c r="B1" s="49"/>
-      <c r="C1" s="49"/>
-      <c r="D1" s="49"/>
-      <c r="E1" s="49"/>
-      <c r="F1" s="49"/>
-      <c r="G1" s="49"/>
-      <c r="H1" s="49"/>
-      <c r="I1" s="49"/>
-      <c r="J1" s="49"/>
-      <c r="K1" s="49"/>
+      <c r="A1" s="45"/>
+      <c r="B1" s="45"/>
+      <c r="C1" s="45"/>
+      <c r="D1" s="45"/>
+      <c r="E1" s="45"/>
+      <c r="F1" s="45"/>
+      <c r="G1" s="45"/>
+      <c r="H1" s="45"/>
+      <c r="I1" s="45"/>
+      <c r="J1" s="45"/>
+      <c r="K1" s="45"/>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A2" s="50"/>
-      <c r="B2" s="50"/>
-      <c r="C2" s="50"/>
-      <c r="D2" s="50"/>
-      <c r="E2" s="50"/>
-      <c r="F2" s="50"/>
-      <c r="G2" s="50"/>
-      <c r="H2" s="50"/>
-      <c r="I2" s="50"/>
-      <c r="J2" s="50"/>
-      <c r="K2" s="50"/>
+      <c r="A2" s="44"/>
+      <c r="B2" s="44"/>
+      <c r="C2" s="44"/>
+      <c r="D2" s="44"/>
+      <c r="E2" s="44"/>
+      <c r="F2" s="44"/>
+      <c r="G2" s="44"/>
+      <c r="H2" s="44"/>
+      <c r="I2" s="44"/>
+      <c r="J2" s="44"/>
+      <c r="K2" s="44"/>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A3" s="46" t="s">
+      <c r="A3" s="37" t="s">
         <v>52</v>
       </c>
-      <c r="B3" s="47"/>
-      <c r="C3" s="47"/>
-      <c r="D3" s="47"/>
-      <c r="E3" s="47"/>
-      <c r="F3" s="47"/>
-      <c r="G3" s="47"/>
-      <c r="H3" s="47"/>
-      <c r="I3" s="47"/>
-      <c r="J3" s="47"/>
-      <c r="K3" s="48"/>
+      <c r="B3" s="38"/>
+      <c r="C3" s="38"/>
+      <c r="D3" s="38"/>
+      <c r="E3" s="38"/>
+      <c r="F3" s="38"/>
+      <c r="G3" s="38"/>
+      <c r="H3" s="38"/>
+      <c r="I3" s="38"/>
+      <c r="J3" s="38"/>
+      <c r="K3" s="39"/>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
@@ -7428,45 +7329,45 @@
       </c>
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A10" s="49"/>
-      <c r="B10" s="49"/>
-      <c r="C10" s="49"/>
-      <c r="D10" s="49"/>
-      <c r="E10" s="49"/>
-      <c r="F10" s="49"/>
-      <c r="G10" s="49"/>
-      <c r="H10" s="49"/>
-      <c r="I10" s="49"/>
-      <c r="J10" s="49"/>
-      <c r="K10" s="49"/>
+      <c r="A10" s="45"/>
+      <c r="B10" s="45"/>
+      <c r="C10" s="45"/>
+      <c r="D10" s="45"/>
+      <c r="E10" s="45"/>
+      <c r="F10" s="45"/>
+      <c r="G10" s="45"/>
+      <c r="H10" s="45"/>
+      <c r="I10" s="45"/>
+      <c r="J10" s="45"/>
+      <c r="K10" s="45"/>
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A11" s="50"/>
-      <c r="B11" s="50"/>
-      <c r="C11" s="50"/>
-      <c r="D11" s="50"/>
-      <c r="E11" s="50"/>
-      <c r="F11" s="50"/>
-      <c r="G11" s="50"/>
-      <c r="H11" s="50"/>
-      <c r="I11" s="50"/>
-      <c r="J11" s="50"/>
-      <c r="K11" s="50"/>
+      <c r="A11" s="44"/>
+      <c r="B11" s="44"/>
+      <c r="C11" s="44"/>
+      <c r="D11" s="44"/>
+      <c r="E11" s="44"/>
+      <c r="F11" s="44"/>
+      <c r="G11" s="44"/>
+      <c r="H11" s="44"/>
+      <c r="I11" s="44"/>
+      <c r="J11" s="44"/>
+      <c r="K11" s="44"/>
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A12" s="46" t="s">
+      <c r="A12" s="37" t="s">
         <v>48</v>
       </c>
-      <c r="B12" s="47"/>
-      <c r="C12" s="47"/>
-      <c r="D12" s="47"/>
-      <c r="E12" s="47"/>
-      <c r="F12" s="47"/>
-      <c r="G12" s="47"/>
-      <c r="H12" s="47"/>
-      <c r="I12" s="47"/>
-      <c r="J12" s="47"/>
-      <c r="K12" s="48"/>
+      <c r="B12" s="38"/>
+      <c r="C12" s="38"/>
+      <c r="D12" s="38"/>
+      <c r="E12" s="38"/>
+      <c r="F12" s="38"/>
+      <c r="G12" s="38"/>
+      <c r="H12" s="38"/>
+      <c r="I12" s="38"/>
+      <c r="J12" s="38"/>
+      <c r="K12" s="39"/>
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A13" s="3" t="s">
@@ -7738,45 +7639,45 @@
       </c>
     </row>
     <row r="22" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A22" s="49"/>
-      <c r="B22" s="49"/>
-      <c r="C22" s="49"/>
-      <c r="D22" s="49"/>
-      <c r="E22" s="49"/>
-      <c r="F22" s="49"/>
-      <c r="G22" s="49"/>
-      <c r="H22" s="49"/>
-      <c r="I22" s="49"/>
-      <c r="J22" s="49"/>
-      <c r="K22" s="49"/>
+      <c r="A22" s="45"/>
+      <c r="B22" s="45"/>
+      <c r="C22" s="45"/>
+      <c r="D22" s="45"/>
+      <c r="E22" s="45"/>
+      <c r="F22" s="45"/>
+      <c r="G22" s="45"/>
+      <c r="H22" s="45"/>
+      <c r="I22" s="45"/>
+      <c r="J22" s="45"/>
+      <c r="K22" s="45"/>
     </row>
     <row r="23" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A23" s="50"/>
-      <c r="B23" s="50"/>
-      <c r="C23" s="50"/>
-      <c r="D23" s="50"/>
-      <c r="E23" s="50"/>
-      <c r="F23" s="50"/>
-      <c r="G23" s="50"/>
-      <c r="H23" s="50"/>
-      <c r="I23" s="50"/>
-      <c r="J23" s="50"/>
-      <c r="K23" s="50"/>
+      <c r="A23" s="44"/>
+      <c r="B23" s="44"/>
+      <c r="C23" s="44"/>
+      <c r="D23" s="44"/>
+      <c r="E23" s="44"/>
+      <c r="F23" s="44"/>
+      <c r="G23" s="44"/>
+      <c r="H23" s="44"/>
+      <c r="I23" s="44"/>
+      <c r="J23" s="44"/>
+      <c r="K23" s="44"/>
     </row>
     <row r="24" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A24" s="46" t="s">
+      <c r="A24" s="37" t="s">
         <v>54</v>
       </c>
-      <c r="B24" s="47"/>
-      <c r="C24" s="47"/>
-      <c r="D24" s="47"/>
-      <c r="E24" s="47"/>
-      <c r="F24" s="47"/>
-      <c r="G24" s="47"/>
-      <c r="H24" s="47"/>
-      <c r="I24" s="47"/>
-      <c r="J24" s="47"/>
-      <c r="K24" s="48"/>
+      <c r="B24" s="38"/>
+      <c r="C24" s="38"/>
+      <c r="D24" s="38"/>
+      <c r="E24" s="38"/>
+      <c r="F24" s="38"/>
+      <c r="G24" s="38"/>
+      <c r="H24" s="38"/>
+      <c r="I24" s="38"/>
+      <c r="J24" s="38"/>
+      <c r="K24" s="39"/>
     </row>
     <row r="25" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A25" s="3" t="s">
@@ -8023,45 +7924,45 @@
       </c>
     </row>
     <row r="33" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A33" s="49"/>
-      <c r="B33" s="49"/>
-      <c r="C33" s="49"/>
-      <c r="D33" s="49"/>
-      <c r="E33" s="49"/>
-      <c r="F33" s="49"/>
-      <c r="G33" s="49"/>
-      <c r="H33" s="49"/>
-      <c r="I33" s="49"/>
-      <c r="J33" s="49"/>
-      <c r="K33" s="49"/>
+      <c r="A33" s="45"/>
+      <c r="B33" s="45"/>
+      <c r="C33" s="45"/>
+      <c r="D33" s="45"/>
+      <c r="E33" s="45"/>
+      <c r="F33" s="45"/>
+      <c r="G33" s="45"/>
+      <c r="H33" s="45"/>
+      <c r="I33" s="45"/>
+      <c r="J33" s="45"/>
+      <c r="K33" s="45"/>
     </row>
     <row r="34" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A34" s="50"/>
-      <c r="B34" s="50"/>
-      <c r="C34" s="50"/>
-      <c r="D34" s="50"/>
-      <c r="E34" s="50"/>
-      <c r="F34" s="50"/>
-      <c r="G34" s="50"/>
-      <c r="H34" s="50"/>
-      <c r="I34" s="50"/>
-      <c r="J34" s="50"/>
-      <c r="K34" s="50"/>
+      <c r="A34" s="44"/>
+      <c r="B34" s="44"/>
+      <c r="C34" s="44"/>
+      <c r="D34" s="44"/>
+      <c r="E34" s="44"/>
+      <c r="F34" s="44"/>
+      <c r="G34" s="44"/>
+      <c r="H34" s="44"/>
+      <c r="I34" s="44"/>
+      <c r="J34" s="44"/>
+      <c r="K34" s="44"/>
     </row>
     <row r="35" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A35" s="46" t="s">
+      <c r="A35" s="37" t="s">
         <v>59</v>
       </c>
-      <c r="B35" s="47"/>
-      <c r="C35" s="47"/>
-      <c r="D35" s="47"/>
-      <c r="E35" s="47"/>
-      <c r="F35" s="47"/>
-      <c r="G35" s="47"/>
-      <c r="H35" s="47"/>
-      <c r="I35" s="47"/>
-      <c r="J35" s="47"/>
-      <c r="K35" s="48"/>
+      <c r="B35" s="38"/>
+      <c r="C35" s="38"/>
+      <c r="D35" s="38"/>
+      <c r="E35" s="38"/>
+      <c r="F35" s="38"/>
+      <c r="G35" s="38"/>
+      <c r="H35" s="38"/>
+      <c r="I35" s="38"/>
+      <c r="J35" s="38"/>
+      <c r="K35" s="39"/>
     </row>
     <row r="36" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A36" s="3" t="s">
@@ -8335,45 +8236,45 @@
       </c>
     </row>
     <row r="45" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A45" s="49"/>
-      <c r="B45" s="49"/>
-      <c r="C45" s="49"/>
-      <c r="D45" s="49"/>
-      <c r="E45" s="49"/>
-      <c r="F45" s="49"/>
-      <c r="G45" s="49"/>
-      <c r="H45" s="49"/>
-      <c r="I45" s="49"/>
-      <c r="J45" s="49"/>
-      <c r="K45" s="49"/>
+      <c r="A45" s="45"/>
+      <c r="B45" s="45"/>
+      <c r="C45" s="45"/>
+      <c r="D45" s="45"/>
+      <c r="E45" s="45"/>
+      <c r="F45" s="45"/>
+      <c r="G45" s="45"/>
+      <c r="H45" s="45"/>
+      <c r="I45" s="45"/>
+      <c r="J45" s="45"/>
+      <c r="K45" s="45"/>
     </row>
     <row r="46" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A46" s="50"/>
-      <c r="B46" s="50"/>
-      <c r="C46" s="50"/>
-      <c r="D46" s="50"/>
-      <c r="E46" s="50"/>
-      <c r="F46" s="50"/>
-      <c r="G46" s="50"/>
-      <c r="H46" s="50"/>
-      <c r="I46" s="50"/>
-      <c r="J46" s="50"/>
-      <c r="K46" s="50"/>
+      <c r="A46" s="44"/>
+      <c r="B46" s="44"/>
+      <c r="C46" s="44"/>
+      <c r="D46" s="44"/>
+      <c r="E46" s="44"/>
+      <c r="F46" s="44"/>
+      <c r="G46" s="44"/>
+      <c r="H46" s="44"/>
+      <c r="I46" s="44"/>
+      <c r="J46" s="44"/>
+      <c r="K46" s="44"/>
     </row>
     <row r="47" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A47" s="46" t="s">
+      <c r="A47" s="37" t="s">
         <v>64</v>
       </c>
-      <c r="B47" s="47"/>
-      <c r="C47" s="47"/>
-      <c r="D47" s="47"/>
-      <c r="E47" s="47"/>
-      <c r="F47" s="47"/>
-      <c r="G47" s="47"/>
-      <c r="H47" s="47"/>
-      <c r="I47" s="47"/>
-      <c r="J47" s="47"/>
-      <c r="K47" s="48"/>
+      <c r="B47" s="38"/>
+      <c r="C47" s="38"/>
+      <c r="D47" s="38"/>
+      <c r="E47" s="38"/>
+      <c r="F47" s="38"/>
+      <c r="G47" s="38"/>
+      <c r="H47" s="38"/>
+      <c r="I47" s="38"/>
+      <c r="J47" s="38"/>
+      <c r="K47" s="39"/>
     </row>
     <row r="48" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A48" s="3" t="s">
@@ -8616,45 +8517,45 @@
       </c>
     </row>
     <row r="56" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A56" s="49"/>
-      <c r="B56" s="49"/>
-      <c r="C56" s="49"/>
-      <c r="D56" s="49"/>
-      <c r="E56" s="49"/>
-      <c r="F56" s="49"/>
-      <c r="G56" s="49"/>
-      <c r="H56" s="49"/>
-      <c r="I56" s="49"/>
-      <c r="J56" s="49"/>
-      <c r="K56" s="49"/>
+      <c r="A56" s="45"/>
+      <c r="B56" s="45"/>
+      <c r="C56" s="45"/>
+      <c r="D56" s="45"/>
+      <c r="E56" s="45"/>
+      <c r="F56" s="45"/>
+      <c r="G56" s="45"/>
+      <c r="H56" s="45"/>
+      <c r="I56" s="45"/>
+      <c r="J56" s="45"/>
+      <c r="K56" s="45"/>
     </row>
     <row r="57" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A57" s="50"/>
-      <c r="B57" s="50"/>
-      <c r="C57" s="50"/>
-      <c r="D57" s="50"/>
-      <c r="E57" s="50"/>
-      <c r="F57" s="50"/>
-      <c r="G57" s="50"/>
-      <c r="H57" s="50"/>
-      <c r="I57" s="50"/>
-      <c r="J57" s="50"/>
-      <c r="K57" s="50"/>
+      <c r="A57" s="44"/>
+      <c r="B57" s="44"/>
+      <c r="C57" s="44"/>
+      <c r="D57" s="44"/>
+      <c r="E57" s="44"/>
+      <c r="F57" s="44"/>
+      <c r="G57" s="44"/>
+      <c r="H57" s="44"/>
+      <c r="I57" s="44"/>
+      <c r="J57" s="44"/>
+      <c r="K57" s="44"/>
     </row>
     <row r="58" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A58" s="46" t="s">
+      <c r="A58" s="37" t="s">
         <v>69</v>
       </c>
-      <c r="B58" s="47"/>
-      <c r="C58" s="47"/>
-      <c r="D58" s="47"/>
-      <c r="E58" s="47"/>
-      <c r="F58" s="47"/>
-      <c r="G58" s="47"/>
-      <c r="H58" s="47"/>
-      <c r="I58" s="47"/>
-      <c r="J58" s="47"/>
-      <c r="K58" s="48"/>
+      <c r="B58" s="38"/>
+      <c r="C58" s="38"/>
+      <c r="D58" s="38"/>
+      <c r="E58" s="38"/>
+      <c r="F58" s="38"/>
+      <c r="G58" s="38"/>
+      <c r="H58" s="38"/>
+      <c r="I58" s="38"/>
+      <c r="J58" s="38"/>
+      <c r="K58" s="39"/>
     </row>
     <row r="59" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A59" s="3" t="s">
@@ -8897,45 +8798,45 @@
       </c>
     </row>
     <row r="67" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A67" s="49"/>
-      <c r="B67" s="49"/>
-      <c r="C67" s="49"/>
-      <c r="D67" s="49"/>
-      <c r="E67" s="49"/>
-      <c r="F67" s="49"/>
-      <c r="G67" s="49"/>
-      <c r="H67" s="49"/>
-      <c r="I67" s="49"/>
-      <c r="J67" s="49"/>
-      <c r="K67" s="49"/>
+      <c r="A67" s="45"/>
+      <c r="B67" s="45"/>
+      <c r="C67" s="45"/>
+      <c r="D67" s="45"/>
+      <c r="E67" s="45"/>
+      <c r="F67" s="45"/>
+      <c r="G67" s="45"/>
+      <c r="H67" s="45"/>
+      <c r="I67" s="45"/>
+      <c r="J67" s="45"/>
+      <c r="K67" s="45"/>
     </row>
     <row r="68" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A68" s="50"/>
-      <c r="B68" s="50"/>
-      <c r="C68" s="50"/>
-      <c r="D68" s="50"/>
-      <c r="E68" s="50"/>
-      <c r="F68" s="50"/>
-      <c r="G68" s="50"/>
-      <c r="H68" s="50"/>
-      <c r="I68" s="50"/>
-      <c r="J68" s="50"/>
-      <c r="K68" s="50"/>
+      <c r="A68" s="44"/>
+      <c r="B68" s="44"/>
+      <c r="C68" s="44"/>
+      <c r="D68" s="44"/>
+      <c r="E68" s="44"/>
+      <c r="F68" s="44"/>
+      <c r="G68" s="44"/>
+      <c r="H68" s="44"/>
+      <c r="I68" s="44"/>
+      <c r="J68" s="44"/>
+      <c r="K68" s="44"/>
     </row>
     <row r="69" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A69" s="46" t="s">
+      <c r="A69" s="37" t="s">
         <v>38</v>
       </c>
-      <c r="B69" s="47"/>
-      <c r="C69" s="47"/>
-      <c r="D69" s="47"/>
-      <c r="E69" s="47"/>
-      <c r="F69" s="47"/>
-      <c r="G69" s="47"/>
-      <c r="H69" s="47"/>
-      <c r="I69" s="47"/>
-      <c r="J69" s="47"/>
-      <c r="K69" s="48"/>
+      <c r="B69" s="38"/>
+      <c r="C69" s="38"/>
+      <c r="D69" s="38"/>
+      <c r="E69" s="38"/>
+      <c r="F69" s="38"/>
+      <c r="G69" s="38"/>
+      <c r="H69" s="38"/>
+      <c r="I69" s="38"/>
+      <c r="J69" s="38"/>
+      <c r="K69" s="39"/>
     </row>
     <row r="70" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A70" s="3" t="s">
@@ -9259,45 +9160,45 @@
       </c>
     </row>
     <row r="82" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A82" s="49"/>
-      <c r="B82" s="49"/>
-      <c r="C82" s="49"/>
-      <c r="D82" s="49"/>
-      <c r="E82" s="49"/>
-      <c r="F82" s="49"/>
-      <c r="G82" s="49"/>
-      <c r="H82" s="49"/>
-      <c r="I82" s="49"/>
-      <c r="J82" s="49"/>
-      <c r="K82" s="49"/>
+      <c r="A82" s="45"/>
+      <c r="B82" s="45"/>
+      <c r="C82" s="45"/>
+      <c r="D82" s="45"/>
+      <c r="E82" s="45"/>
+      <c r="F82" s="45"/>
+      <c r="G82" s="45"/>
+      <c r="H82" s="45"/>
+      <c r="I82" s="45"/>
+      <c r="J82" s="45"/>
+      <c r="K82" s="45"/>
     </row>
     <row r="83" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A83" s="50"/>
-      <c r="B83" s="50"/>
-      <c r="C83" s="50"/>
-      <c r="D83" s="50"/>
-      <c r="E83" s="50"/>
-      <c r="F83" s="50"/>
-      <c r="G83" s="50"/>
-      <c r="H83" s="50"/>
-      <c r="I83" s="50"/>
-      <c r="J83" s="50"/>
-      <c r="K83" s="50"/>
+      <c r="A83" s="44"/>
+      <c r="B83" s="44"/>
+      <c r="C83" s="44"/>
+      <c r="D83" s="44"/>
+      <c r="E83" s="44"/>
+      <c r="F83" s="44"/>
+      <c r="G83" s="44"/>
+      <c r="H83" s="44"/>
+      <c r="I83" s="44"/>
+      <c r="J83" s="44"/>
+      <c r="K83" s="44"/>
     </row>
     <row r="84" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A84" s="46" t="s">
+      <c r="A84" s="37" t="s">
         <v>76</v>
       </c>
-      <c r="B84" s="47"/>
-      <c r="C84" s="47"/>
-      <c r="D84" s="47"/>
-      <c r="E84" s="47"/>
-      <c r="F84" s="47"/>
-      <c r="G84" s="47"/>
-      <c r="H84" s="47"/>
-      <c r="I84" s="47"/>
-      <c r="J84" s="47"/>
-      <c r="K84" s="48"/>
+      <c r="B84" s="38"/>
+      <c r="C84" s="38"/>
+      <c r="D84" s="38"/>
+      <c r="E84" s="38"/>
+      <c r="F84" s="38"/>
+      <c r="G84" s="38"/>
+      <c r="H84" s="38"/>
+      <c r="I84" s="38"/>
+      <c r="J84" s="38"/>
+      <c r="K84" s="39"/>
     </row>
     <row r="85" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A85" s="19" t="s">
@@ -9478,45 +9379,45 @@
       </c>
     </row>
     <row r="91" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A91" s="49"/>
-      <c r="B91" s="49"/>
-      <c r="C91" s="49"/>
-      <c r="D91" s="49"/>
-      <c r="E91" s="49"/>
-      <c r="F91" s="49"/>
-      <c r="G91" s="49"/>
-      <c r="H91" s="49"/>
-      <c r="I91" s="49"/>
-      <c r="J91" s="49"/>
-      <c r="K91" s="49"/>
+      <c r="A91" s="45"/>
+      <c r="B91" s="45"/>
+      <c r="C91" s="45"/>
+      <c r="D91" s="45"/>
+      <c r="E91" s="45"/>
+      <c r="F91" s="45"/>
+      <c r="G91" s="45"/>
+      <c r="H91" s="45"/>
+      <c r="I91" s="45"/>
+      <c r="J91" s="45"/>
+      <c r="K91" s="45"/>
     </row>
     <row r="92" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A92" s="50"/>
-      <c r="B92" s="50"/>
-      <c r="C92" s="50"/>
-      <c r="D92" s="50"/>
-      <c r="E92" s="50"/>
-      <c r="F92" s="50"/>
-      <c r="G92" s="50"/>
-      <c r="H92" s="50"/>
-      <c r="I92" s="50"/>
-      <c r="J92" s="50"/>
-      <c r="K92" s="50"/>
+      <c r="A92" s="44"/>
+      <c r="B92" s="44"/>
+      <c r="C92" s="44"/>
+      <c r="D92" s="44"/>
+      <c r="E92" s="44"/>
+      <c r="F92" s="44"/>
+      <c r="G92" s="44"/>
+      <c r="H92" s="44"/>
+      <c r="I92" s="44"/>
+      <c r="J92" s="44"/>
+      <c r="K92" s="44"/>
     </row>
     <row r="93" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A93" s="46" t="s">
+      <c r="A93" s="37" t="s">
         <v>75</v>
       </c>
-      <c r="B93" s="47"/>
-      <c r="C93" s="47"/>
-      <c r="D93" s="47"/>
-      <c r="E93" s="47"/>
-      <c r="F93" s="47"/>
-      <c r="G93" s="47"/>
-      <c r="H93" s="47"/>
-      <c r="I93" s="47"/>
-      <c r="J93" s="47"/>
-      <c r="K93" s="48"/>
+      <c r="B93" s="38"/>
+      <c r="C93" s="38"/>
+      <c r="D93" s="38"/>
+      <c r="E93" s="38"/>
+      <c r="F93" s="38"/>
+      <c r="G93" s="38"/>
+      <c r="H93" s="38"/>
+      <c r="I93" s="38"/>
+      <c r="J93" s="38"/>
+      <c r="K93" s="39"/>
     </row>
     <row r="94" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A94" s="3" t="s">
@@ -9763,45 +9664,45 @@
       </c>
     </row>
     <row r="103" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A103" s="49"/>
-      <c r="B103" s="49"/>
-      <c r="C103" s="49"/>
-      <c r="D103" s="49"/>
-      <c r="E103" s="49"/>
-      <c r="F103" s="49"/>
-      <c r="G103" s="49"/>
-      <c r="H103" s="49"/>
-      <c r="I103" s="49"/>
-      <c r="J103" s="49"/>
-      <c r="K103" s="49"/>
+      <c r="A103" s="45"/>
+      <c r="B103" s="45"/>
+      <c r="C103" s="45"/>
+      <c r="D103" s="45"/>
+      <c r="E103" s="45"/>
+      <c r="F103" s="45"/>
+      <c r="G103" s="45"/>
+      <c r="H103" s="45"/>
+      <c r="I103" s="45"/>
+      <c r="J103" s="45"/>
+      <c r="K103" s="45"/>
     </row>
     <row r="104" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A104" s="50"/>
-      <c r="B104" s="50"/>
-      <c r="C104" s="50"/>
-      <c r="D104" s="50"/>
-      <c r="E104" s="50"/>
-      <c r="F104" s="50"/>
-      <c r="G104" s="50"/>
-      <c r="H104" s="50"/>
-      <c r="I104" s="50"/>
-      <c r="J104" s="50"/>
-      <c r="K104" s="50"/>
+      <c r="A104" s="44"/>
+      <c r="B104" s="44"/>
+      <c r="C104" s="44"/>
+      <c r="D104" s="44"/>
+      <c r="E104" s="44"/>
+      <c r="F104" s="44"/>
+      <c r="G104" s="44"/>
+      <c r="H104" s="44"/>
+      <c r="I104" s="44"/>
+      <c r="J104" s="44"/>
+      <c r="K104" s="44"/>
     </row>
     <row r="105" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A105" s="46" t="s">
+      <c r="A105" s="37" t="s">
         <v>33</v>
       </c>
-      <c r="B105" s="47"/>
-      <c r="C105" s="47"/>
-      <c r="D105" s="47"/>
-      <c r="E105" s="47"/>
-      <c r="F105" s="47"/>
-      <c r="G105" s="47"/>
-      <c r="H105" s="47"/>
-      <c r="I105" s="47"/>
-      <c r="J105" s="47"/>
-      <c r="K105" s="48"/>
+      <c r="B105" s="38"/>
+      <c r="C105" s="38"/>
+      <c r="D105" s="38"/>
+      <c r="E105" s="38"/>
+      <c r="F105" s="38"/>
+      <c r="G105" s="38"/>
+      <c r="H105" s="38"/>
+      <c r="I105" s="38"/>
+      <c r="J105" s="38"/>
+      <c r="K105" s="39"/>
     </row>
     <row r="106" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A106" s="19" t="s">
@@ -9932,45 +9833,45 @@
       <c r="K109" s="14"/>
     </row>
     <row r="110" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A110" s="49"/>
-      <c r="B110" s="49"/>
-      <c r="C110" s="49"/>
-      <c r="D110" s="49"/>
-      <c r="E110" s="49"/>
-      <c r="F110" s="49"/>
-      <c r="G110" s="49"/>
-      <c r="H110" s="49"/>
-      <c r="I110" s="49"/>
-      <c r="J110" s="49"/>
-      <c r="K110" s="49"/>
+      <c r="A110" s="45"/>
+      <c r="B110" s="45"/>
+      <c r="C110" s="45"/>
+      <c r="D110" s="45"/>
+      <c r="E110" s="45"/>
+      <c r="F110" s="45"/>
+      <c r="G110" s="45"/>
+      <c r="H110" s="45"/>
+      <c r="I110" s="45"/>
+      <c r="J110" s="45"/>
+      <c r="K110" s="45"/>
     </row>
     <row r="111" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A111" s="50"/>
-      <c r="B111" s="50"/>
-      <c r="C111" s="50"/>
-      <c r="D111" s="50"/>
-      <c r="E111" s="50"/>
-      <c r="F111" s="50"/>
-      <c r="G111" s="50"/>
-      <c r="H111" s="50"/>
-      <c r="I111" s="50"/>
-      <c r="J111" s="50"/>
-      <c r="K111" s="50"/>
+      <c r="A111" s="44"/>
+      <c r="B111" s="44"/>
+      <c r="C111" s="44"/>
+      <c r="D111" s="44"/>
+      <c r="E111" s="44"/>
+      <c r="F111" s="44"/>
+      <c r="G111" s="44"/>
+      <c r="H111" s="44"/>
+      <c r="I111" s="44"/>
+      <c r="J111" s="44"/>
+      <c r="K111" s="44"/>
     </row>
     <row r="112" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A112" s="46" t="s">
+      <c r="A112" s="37" t="s">
         <v>35</v>
       </c>
-      <c r="B112" s="47"/>
-      <c r="C112" s="47"/>
-      <c r="D112" s="47"/>
-      <c r="E112" s="47"/>
-      <c r="F112" s="47"/>
-      <c r="G112" s="47"/>
-      <c r="H112" s="47"/>
-      <c r="I112" s="47"/>
-      <c r="J112" s="47"/>
-      <c r="K112" s="48"/>
+      <c r="B112" s="38"/>
+      <c r="C112" s="38"/>
+      <c r="D112" s="38"/>
+      <c r="E112" s="38"/>
+      <c r="F112" s="38"/>
+      <c r="G112" s="38"/>
+      <c r="H112" s="38"/>
+      <c r="I112" s="38"/>
+      <c r="J112" s="38"/>
+      <c r="K112" s="39"/>
     </row>
     <row r="113" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A113" s="19" t="s">

</xml_diff>